<commit_message>
added end dates to SIP data
</commit_message>
<xml_diff>
--- a/Data/SIP-weeks-by-state.xlsx
+++ b/Data/SIP-weeks-by-state.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corinneriddell/Documents/repos/SIP-and-abuse/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{409A7859-9B49-554B-8AC4-1150CB24864E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FBE20E6F-F13A-954B-B501-BE47990A5FFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{1B9F9A4B-0140-2A4C-9F74-A2DD557B0179}"/>
+    <workbookView xWindow="-47460" yWindow="-12240" windowWidth="34780" windowHeight="24060" xr2:uid="{1B9F9A4B-0140-2A4C-9F74-A2DD557B0179}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>AL</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t>Ever_txt</t>
+  </si>
+  <si>
+    <t>Wk_SIP_end</t>
   </si>
 </sst>
 </file>
@@ -184,12 +187,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -204,8 +213,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -520,18 +530,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ECEC5F4-76C6-4297-A7E0-219552290DAE}">
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:E1048576"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>42</v>
       </c>
@@ -541,8 +552,11 @@
       <c r="C1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -552,8 +566,11 @@
       <c r="C2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -563,8 +580,11 @@
       <c r="C3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -574,8 +594,11 @@
       <c r="C4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -585,8 +608,11 @@
       <c r="C5">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -596,8 +622,11 @@
       <c r="C6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -607,8 +636,11 @@
       <c r="C7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -618,8 +650,11 @@
       <c r="C8">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D8">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -629,8 +664,11 @@
       <c r="C9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -640,8 +678,11 @@
       <c r="C10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -651,8 +692,11 @@
       <c r="C11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -662,8 +706,11 @@
       <c r="C12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -673,8 +720,11 @@
       <c r="C13">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D13">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -684,8 +734,11 @@
       <c r="C14">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D14">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -695,8 +748,11 @@
       <c r="C15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D15">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -706,8 +762,11 @@
       <c r="C16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -717,8 +776,11 @@
       <c r="C17">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -728,8 +790,11 @@
       <c r="C18">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -739,8 +804,11 @@
       <c r="C19">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -750,8 +818,11 @@
       <c r="C20">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -761,8 +832,11 @@
       <c r="C21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D21">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -772,8 +846,11 @@
       <c r="C22">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -783,8 +860,11 @@
       <c r="C23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D23">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -794,8 +874,11 @@
       <c r="C24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D24">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -805,8 +888,11 @@
       <c r="C25">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -816,8 +902,11 @@
       <c r="C26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -827,8 +916,11 @@
       <c r="C27">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D27">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -838,8 +930,11 @@
       <c r="C28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D28">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -849,8 +944,11 @@
       <c r="C29">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D29">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -860,19 +958,25 @@
       <c r="C30">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D30">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>28</v>
       </c>
-      <c r="B31">
-        <v>13</v>
+      <c r="B31" s="1">
+        <v>12</v>
       </c>
       <c r="C31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D31">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -882,19 +986,25 @@
       <c r="C32">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="D32">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B33">
-        <v>0</v>
-      </c>
-      <c r="C33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B33" s="1">
+        <v>14</v>
+      </c>
+      <c r="C33" s="1">
+        <v>1</v>
+      </c>
+      <c r="D33" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -904,8 +1014,11 @@
       <c r="C34">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D34">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -915,8 +1028,11 @@
       <c r="C35">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D35">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -926,8 +1042,11 @@
       <c r="C36">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D36">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -937,8 +1056,11 @@
       <c r="C37">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D37">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -948,8 +1070,11 @@
       <c r="C38">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D38">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -959,8 +1084,11 @@
       <c r="C39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -970,8 +1098,11 @@
       <c r="C40">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D40">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -981,8 +1112,11 @@
       <c r="C41">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D41">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -992,8 +1126,11 @@
       <c r="C42">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D42">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>40</v>
       </c>
@@ -1002,6 +1139,9 @@
       </c>
       <c r="C43">
         <v>1</v>
+      </c>
+      <c r="D43">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add weak vs strong ban info
</commit_message>
<xml_diff>
--- a/Data/SIP-weeks-by-state.xlsx
+++ b/Data/SIP-weeks-by-state.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/corinneriddell/Documents/repos/SIP-and-abuse/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FBE20E6F-F13A-954B-B501-BE47990A5FFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7807AD5-D409-FC49-8A55-ABE5346B41BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-47460" yWindow="-12240" windowWidth="34780" windowHeight="24060" xr2:uid="{1B9F9A4B-0140-2A4C-9F74-A2DD557B0179}"/>
+    <workbookView xWindow="-53940" yWindow="-13220" windowWidth="14260" windowHeight="24060" xr2:uid="{1B9F9A4B-0140-2A4C-9F74-A2DD557B0179}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>AL</t>
   </si>
@@ -172,19 +172,43 @@
   </si>
   <si>
     <t>Wk_SIP_end</t>
+  </si>
+  <si>
+    <t>Weak_ban</t>
+  </si>
+  <si>
+    <t>CT - "Stay Safe, Stay Home" order does not have any language that orders individuals to stay at home; 3/23/2020 safer-at-home order acted only to close nonessential businesses</t>
+  </si>
+  <si>
+    <t>GA - Only high-risk individuals were ordered to shelter in place</t>
+  </si>
+  <si>
+    <t>KY - Order on 3/25/2020 did not have any language ordering individuals to stay at home; 3/26/2020 order did not order residents to stay at home; Order never applied to the entire state but it expired officially on 6/29/2020</t>
+  </si>
+  <si>
+    <t>OK - Stay-at-home order from 4/1 only applied to those over 65; order was allowed to expire 5/15 per state's website</t>
+  </si>
+  <si>
+    <t>TX - Stay-at-home order issued 4/2, though it does not explicitly order individuals to stay at home</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -213,9 +237,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -530,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ECEC5F4-76C6-4297-A7E0-219552290DAE}">
-  <dimension ref="A1:D43"/>
+  <dimension ref="A1:F43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -542,7 +567,7 @@
     <col min="4" max="4" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>42</v>
       </c>
@@ -555,8 +580,11 @@
       <c r="D1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -569,8 +597,11 @@
       <c r="D2">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -583,8 +614,11 @@
       <c r="D3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -597,8 +631,11 @@
       <c r="D4">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -611,8 +648,11 @@
       <c r="D5">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -625,8 +665,11 @@
       <c r="D6">
         <v>18</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -639,8 +682,14 @@
       <c r="D7">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -653,8 +702,11 @@
       <c r="D8">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -667,8 +719,14 @@
       <c r="D9">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -681,8 +739,11 @@
       <c r="D10">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -695,8 +756,11 @@
       <c r="D11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -709,8 +773,11 @@
       <c r="D12">
         <v>18</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -723,8 +790,11 @@
       <c r="D13">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -737,8 +807,11 @@
       <c r="D14">
         <v>21</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -751,8 +824,11 @@
       <c r="D15">
         <v>19</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -765,8 +841,14 @@
       <c r="D16">
         <v>24</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -779,8 +861,11 @@
       <c r="D17">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -793,8 +878,11 @@
       <c r="D18">
         <v>21</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -807,8 +895,11 @@
       <c r="D19">
         <v>20</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -821,8 +912,11 @@
       <c r="D20">
         <v>22</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -835,8 +929,11 @@
       <c r="D21">
         <v>23</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -849,8 +946,11 @@
       <c r="D22">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -863,8 +963,11 @@
       <c r="D23">
         <v>19</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -877,8 +980,11 @@
       <c r="D24">
         <v>18</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -891,8 +997,11 @@
       <c r="D25">
         <v>21</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -905,8 +1014,11 @@
       <c r="D26">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -919,8 +1031,11 @@
       <c r="D27">
         <v>24</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -933,8 +1048,11 @@
       <c r="D28">
         <v>24</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -947,8 +1065,11 @@
       <c r="D29">
         <v>24</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>24</v>
       </c>
@@ -961,8 +1082,11 @@
       <c r="D30">
         <v>19</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>28</v>
       </c>
@@ -975,8 +1099,11 @@
       <c r="D31">
         <v>24</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -989,8 +1116,11 @@
       <c r="D32">
         <v>21</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
@@ -1003,8 +1133,14 @@
       <c r="D33" s="1">
         <v>20</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E33" s="1">
+        <v>1</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1017,8 +1153,11 @@
       <c r="D34">
         <v>24</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1031,8 +1170,11 @@
       <c r="D35">
         <v>23</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -1045,8 +1187,11 @@
       <c r="D36">
         <v>19</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -1059,8 +1204,11 @@
       <c r="D37">
         <v>18</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -1073,8 +1221,14 @@
       <c r="D38">
         <v>18</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E38">
+        <v>1</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -1087,8 +1241,11 @@
       <c r="D39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -1101,8 +1258,11 @@
       <c r="D40">
         <v>22</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -1115,8 +1275,11 @@
       <c r="D41">
         <v>23</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -1129,8 +1292,11 @@
       <c r="D42">
         <v>20</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>40</v>
       </c>
@@ -1142,6 +1308,9 @@
       </c>
       <c r="D43">
         <v>19</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>